<commit_message>
Reporte de Medicion v1 - gestionarevaluacion
</commit_message>
<xml_diff>
--- a/gestionarEvaluacion/Resource/template.xlsx
+++ b/gestionarEvaluacion/Resource/template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Escritorio\Redes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\OneDrive\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F207269E-5190-4CBA-95F6-EE06096B7B2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E59208A-654A-495F-83C2-7648A691EDC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
     <author>bcardenas</author>
   </authors>
   <commentList>
-    <comment ref="J7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
+    <comment ref="K7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>PONTIFICIA UNIVERSIDAD CATÓLICA DEL PERÚ</t>
   </si>
@@ -107,12 +107,18 @@
   <si>
     <t>1.2                Evalúa alternativas de solución</t>
   </si>
+  <si>
+    <t>Horario:</t>
+  </si>
+  <si>
+    <t>Tipo de Medición:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,6 +177,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -698,7 +711,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -716,8 +729,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="6" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="6" applyFill="1" applyBorder="1"/>
@@ -750,10 +764,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -780,20 +790,45 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -804,24 +839,83 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="39" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="34" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="35" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="36" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="25" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="9" xfId="17" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="4" xfId="17" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="18" xfId="17" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="39" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -841,81 +935,38 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="39" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="34" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="35" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="36" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="25" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="18">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 10" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal 11" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
@@ -933,6 +984,7 @@
     <cellStyle name="Normal 7" xfId="13" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
     <cellStyle name="Normal 8" xfId="14" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
     <cellStyle name="Normal 9" xfId="15" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Porcentaje" xfId="17" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -951,14 +1003,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>400050</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>1165972</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>574268</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
@@ -1426,330 +1478,332 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="B1:Q36"/>
+  <dimension ref="B1:Q110"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="E17" sqref="E17:H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" style="23" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" style="23" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="23" customWidth="1"/>
-    <col min="4" max="4" width="53.140625" style="23" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" style="23" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" style="23" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" style="23" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" style="23" customWidth="1"/>
-    <col min="9" max="9" width="16" style="23" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" style="23" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" style="23" customWidth="1"/>
-    <col min="12" max="13" width="15" style="23" customWidth="1"/>
-    <col min="14" max="15" width="16.42578125" style="23" customWidth="1"/>
-    <col min="16" max="16" width="19.140625" style="23" customWidth="1"/>
-    <col min="17" max="17" width="23.7109375" style="23" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" style="23" customWidth="1"/>
-    <col min="19" max="16384" width="11.42578125" style="23"/>
+    <col min="1" max="1" width="5.85546875" style="21" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" style="21" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="21" customWidth="1"/>
+    <col min="4" max="4" width="53.140625" style="21" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" style="21" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" style="21" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" style="21" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" style="21" customWidth="1"/>
+    <col min="9" max="9" width="16" style="21" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" style="21" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" style="21" customWidth="1"/>
+    <col min="12" max="13" width="15" style="21" customWidth="1"/>
+    <col min="14" max="15" width="16.42578125" style="21" customWidth="1"/>
+    <col min="16" max="16" width="19.140625" style="21" customWidth="1"/>
+    <col min="17" max="17" width="23.7109375" style="21" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="21" customWidth="1"/>
+    <col min="19" max="16384" width="11.42578125" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:17" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="36"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="42" t="s">
+      <c r="B2" s="39"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="17" t="s">
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="15" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="2:17" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="39"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="43" t="s">
+      <c r="B3" s="42"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31"/>
-      <c r="L3" s="31"/>
-      <c r="M3" s="31"/>
-      <c r="N3" s="31"/>
-      <c r="O3" s="31"/>
-      <c r="P3" s="31"/>
-      <c r="Q3" s="18" t="s">
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="49"/>
+      <c r="Q3" s="16" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:17" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="26"/>
+      <c r="C5" s="53"/>
       <c r="D5" s="10" t="s">
         <v>5</v>
       </c>
       <c r="E5" s="3"/>
-      <c r="F5" s="6"/>
-      <c r="H5" s="62" t="s">
+      <c r="F5" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="I5" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="63"/>
-      <c r="J5" s="2"/>
+      <c r="J5" s="64"/>
       <c r="K5" s="2"/>
-      <c r="L5" s="6"/>
-      <c r="N5" s="44"/>
-      <c r="O5" s="22"/>
-      <c r="P5" s="22"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="6"/>
+      <c r="O5" s="50"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="20"/>
     </row>
     <row r="6" spans="2:17" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="8"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="7"/>
-      <c r="H6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="7"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
-      <c r="N6" s="33"/>
+      <c r="L6" s="1"/>
+      <c r="O6" s="51"/>
     </row>
     <row r="7" spans="2:17" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="26"/>
+      <c r="C7" s="53"/>
       <c r="D7" s="9"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="21" t="s">
+      <c r="F7" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="47" t="s">
+      <c r="I7" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="48"/>
-      <c r="J7" s="53"/>
+      <c r="J7" s="74"/>
       <c r="K7" s="54"/>
       <c r="L7" s="55"/>
-      <c r="N7" s="33"/>
+      <c r="M7" s="56"/>
+      <c r="O7" s="51"/>
     </row>
     <row r="8" spans="2:17" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="8"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="19"/>
-      <c r="H8" s="49"/>
-      <c r="I8" s="50"/>
-      <c r="J8" s="56"/>
+      <c r="F8" s="17"/>
+      <c r="I8" s="75"/>
+      <c r="J8" s="76"/>
       <c r="K8" s="57"/>
       <c r="L8" s="58"/>
+      <c r="M8" s="59"/>
     </row>
     <row r="9" spans="2:17" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="20"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="52"/>
-      <c r="J9" s="59"/>
+      <c r="F9" s="18"/>
+      <c r="I9" s="77"/>
+      <c r="J9" s="78"/>
       <c r="K9" s="60"/>
       <c r="L9" s="61"/>
+      <c r="M9" s="62"/>
     </row>
     <row r="10" spans="2:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="20"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="24"/>
+      <c r="F10" s="18"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
     </row>
     <row r="11" spans="2:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="24"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
     </row>
     <row r="12" spans="2:17" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
     </row>
     <row r="13" spans="2:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="25"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="23"/>
     </row>
     <row r="14" spans="2:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E14" s="45" t="s">
+      <c r="E14" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="64"/>
-      <c r="G14" s="64"/>
-      <c r="H14" s="46"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="25"/>
-      <c r="L14" s="25"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="23"/>
     </row>
     <row r="15" spans="2:17" ht="133.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="41" t="s">
+      <c r="B15" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="65" t="s">
+      <c r="C15" s="46"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="66"/>
-      <c r="G15" s="66"/>
-      <c r="H15" s="67"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="25"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="68" t="e">
-        <f>AVERAGE(E25:E25)</f>
-        <v>#DIV/0!</v>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="86">
+        <v>2</v>
       </c>
-      <c r="F16" s="69"/>
-      <c r="G16" s="69"/>
-      <c r="H16" s="70"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="25"/>
-      <c r="L16" s="25"/>
+      <c r="F16" s="87"/>
+      <c r="G16" s="87"/>
+      <c r="H16" s="88"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="71" t="e">
-        <f>#REF!/E18</f>
-        <v>#REF!</v>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="65">
+        <v>0.1</v>
       </c>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="72"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="25"/>
-      <c r="L17" s="25"/>
+      <c r="F17" s="66"/>
+      <c r="G17" s="66"/>
+      <c r="H17" s="67"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="23"/>
     </row>
     <row r="18" spans="2:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="73">
-        <f>COUNT($C$25:$C$25)</f>
-        <v>0</v>
-      </c>
-      <c r="F18" s="74"/>
-      <c r="G18" s="74"/>
-      <c r="H18" s="75"/>
-      <c r="I18" s="25"/>
-      <c r="J18" s="25"/>
-      <c r="K18" s="25"/>
-      <c r="L18" s="25"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="68"/>
+      <c r="F18" s="69"/>
+      <c r="G18" s="69"/>
+      <c r="H18" s="70"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="23"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="25"/>
-      <c r="K19" s="25"/>
-      <c r="L19" s="25"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="25"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="25"/>
-      <c r="L20" s="25"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="25"/>
-      <c r="L21" s="25"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="23"/>
     </row>
     <row r="22" spans="2:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E22" s="76"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="25"/>
-      <c r="I22" s="25"/>
-      <c r="J22" s="25"/>
-      <c r="K22" s="25"/>
-      <c r="L22" s="25"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="23"/>
     </row>
     <row r="23" spans="2:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E23" s="45" t="s">
+      <c r="E23" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="F23" s="64"/>
-      <c r="G23" s="64"/>
-      <c r="H23" s="46"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="25"/>
-      <c r="K23" s="25"/>
-      <c r="L23" s="25"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23"/>
     </row>
     <row r="24" spans="2:12" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="11" t="s">
@@ -1761,131 +1815,919 @@
       <c r="D24" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E24" s="65" t="s">
+      <c r="E24" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="F24" s="66"/>
-      <c r="G24" s="66"/>
-      <c r="H24" s="67"/>
-      <c r="I24" s="25"/>
-      <c r="J24" s="25"/>
-      <c r="K24" s="25"/>
-      <c r="L24" s="25"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="23"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="14"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="77"/>
-      <c r="E25" s="68"/>
-      <c r="F25" s="69"/>
-      <c r="G25" s="69"/>
-      <c r="H25" s="70"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="25"/>
-      <c r="K25" s="25"/>
-      <c r="L25" s="25"/>
+      <c r="B25" s="79"/>
+      <c r="C25" s="80"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="81"/>
+      <c r="F25" s="82"/>
+      <c r="G25" s="82"/>
+      <c r="H25" s="83"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="23"/>
+      <c r="L25" s="23"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="25"/>
-      <c r="K26" s="25"/>
-      <c r="L26" s="25"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="84"/>
+      <c r="F26" s="84"/>
+      <c r="G26" s="84"/>
+      <c r="H26" s="84"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="23"/>
+      <c r="K26" s="23"/>
+      <c r="L26" s="23"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="25"/>
-      <c r="J27" s="25"/>
-      <c r="K27" s="25"/>
-      <c r="L27" s="25"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="85"/>
+      <c r="F27" s="85"/>
+      <c r="G27" s="85"/>
+      <c r="H27" s="85"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="23"/>
+      <c r="K27" s="23"/>
+      <c r="L27" s="23"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
-      <c r="K28" s="25"/>
-      <c r="L28" s="25"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="85"/>
+      <c r="F28" s="85"/>
+      <c r="G28" s="85"/>
+      <c r="H28" s="85"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
+      <c r="K28" s="23"/>
+      <c r="L28" s="23"/>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
-      <c r="K29" s="25"/>
-      <c r="L29" s="25"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="85"/>
+      <c r="F29" s="85"/>
+      <c r="G29" s="85"/>
+      <c r="H29" s="85"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="23"/>
+      <c r="K29" s="23"/>
+      <c r="L29" s="23"/>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F30" s="25"/>
-      <c r="G30" s="25"/>
-      <c r="H30" s="25"/>
-      <c r="I30" s="25"/>
-      <c r="J30" s="25"/>
-      <c r="K30" s="25"/>
-      <c r="L30" s="25"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="85"/>
+      <c r="F30" s="85"/>
+      <c r="G30" s="85"/>
+      <c r="H30" s="85"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="23"/>
+      <c r="K30" s="23"/>
+      <c r="L30" s="23"/>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
-      <c r="H31" s="25"/>
-      <c r="I31" s="25"/>
-      <c r="J31" s="25"/>
-      <c r="K31" s="25"/>
-      <c r="L31" s="25"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="85"/>
+      <c r="F31" s="85"/>
+      <c r="G31" s="85"/>
+      <c r="H31" s="85"/>
+      <c r="I31" s="23"/>
+      <c r="J31" s="23"/>
+      <c r="K31" s="23"/>
+      <c r="L31" s="23"/>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F32" s="25"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="25"/>
-      <c r="I32" s="25"/>
-      <c r="J32" s="25"/>
-      <c r="K32" s="25"/>
-      <c r="L32" s="25"/>
-    </row>
-    <row r="33" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
-      <c r="H33" s="25"/>
-      <c r="I33" s="25"/>
-      <c r="J33" s="25"/>
-      <c r="K33" s="25"/>
-      <c r="L33" s="25"/>
-    </row>
-    <row r="34" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F34" s="25"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="25"/>
-      <c r="I34" s="25"/>
-      <c r="J34" s="25"/>
-      <c r="K34" s="25"/>
-      <c r="L34" s="25"/>
-    </row>
-    <row r="35" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F35" s="25"/>
-      <c r="G35" s="25"/>
-      <c r="H35" s="25"/>
-      <c r="I35" s="25"/>
-      <c r="J35" s="25"/>
-      <c r="K35" s="25"/>
-      <c r="L35" s="25"/>
-    </row>
-    <row r="36" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F36" s="25"/>
-      <c r="G36" s="25"/>
-      <c r="H36" s="25"/>
-      <c r="I36" s="25"/>
-      <c r="J36" s="25"/>
-      <c r="K36" s="25"/>
-      <c r="L36" s="25"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="85"/>
+      <c r="F32" s="85"/>
+      <c r="G32" s="85"/>
+      <c r="H32" s="85"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="23"/>
+      <c r="K32" s="23"/>
+      <c r="L32" s="23"/>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B33" s="29"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="85"/>
+      <c r="F33" s="85"/>
+      <c r="G33" s="85"/>
+      <c r="H33" s="85"/>
+      <c r="I33" s="23"/>
+      <c r="J33" s="23"/>
+      <c r="K33" s="23"/>
+      <c r="L33" s="23"/>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B34" s="29"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="85"/>
+      <c r="F34" s="85"/>
+      <c r="G34" s="85"/>
+      <c r="H34" s="85"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="23"/>
+      <c r="K34" s="23"/>
+      <c r="L34" s="23"/>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B35" s="29"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="85"/>
+      <c r="F35" s="85"/>
+      <c r="G35" s="85"/>
+      <c r="H35" s="85"/>
+      <c r="I35" s="23"/>
+      <c r="J35" s="23"/>
+      <c r="K35" s="23"/>
+      <c r="L35" s="23"/>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B36" s="29"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="29"/>
+      <c r="E36" s="85"/>
+      <c r="F36" s="85"/>
+      <c r="G36" s="85"/>
+      <c r="H36" s="85"/>
+      <c r="I36" s="23"/>
+      <c r="J36" s="23"/>
+      <c r="K36" s="23"/>
+      <c r="L36" s="23"/>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B37" s="29"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="29"/>
+      <c r="E37" s="85"/>
+      <c r="F37" s="85"/>
+      <c r="G37" s="85"/>
+      <c r="H37" s="85"/>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B38" s="29"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="29"/>
+      <c r="E38" s="85"/>
+      <c r="F38" s="85"/>
+      <c r="G38" s="85"/>
+      <c r="H38" s="85"/>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B39" s="29"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="29"/>
+      <c r="E39" s="85"/>
+      <c r="F39" s="85"/>
+      <c r="G39" s="85"/>
+      <c r="H39" s="85"/>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B40" s="29"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="29"/>
+      <c r="E40" s="85"/>
+      <c r="F40" s="85"/>
+      <c r="G40" s="85"/>
+      <c r="H40" s="85"/>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B41" s="29"/>
+      <c r="C41" s="29"/>
+      <c r="D41" s="29"/>
+      <c r="E41" s="85"/>
+      <c r="F41" s="85"/>
+      <c r="G41" s="85"/>
+      <c r="H41" s="85"/>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B42" s="29"/>
+      <c r="C42" s="29"/>
+      <c r="D42" s="29"/>
+      <c r="E42" s="85"/>
+      <c r="F42" s="85"/>
+      <c r="G42" s="85"/>
+      <c r="H42" s="85"/>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B43" s="29"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="85"/>
+      <c r="F43" s="85"/>
+      <c r="G43" s="85"/>
+      <c r="H43" s="85"/>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B44" s="29"/>
+      <c r="C44" s="29"/>
+      <c r="D44" s="29"/>
+      <c r="E44" s="85"/>
+      <c r="F44" s="85"/>
+      <c r="G44" s="85"/>
+      <c r="H44" s="85"/>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B45" s="29"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="85"/>
+      <c r="F45" s="85"/>
+      <c r="G45" s="85"/>
+      <c r="H45" s="85"/>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B46" s="29"/>
+      <c r="C46" s="29"/>
+      <c r="D46" s="29"/>
+      <c r="E46" s="85"/>
+      <c r="F46" s="85"/>
+      <c r="G46" s="85"/>
+      <c r="H46" s="85"/>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B47" s="29"/>
+      <c r="C47" s="29"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="85"/>
+      <c r="F47" s="85"/>
+      <c r="G47" s="85"/>
+      <c r="H47" s="85"/>
+    </row>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B48" s="29"/>
+      <c r="C48" s="29"/>
+      <c r="D48" s="29"/>
+      <c r="E48" s="85"/>
+      <c r="F48" s="85"/>
+      <c r="G48" s="85"/>
+      <c r="H48" s="85"/>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B49" s="29"/>
+      <c r="C49" s="29"/>
+      <c r="D49" s="29"/>
+      <c r="E49" s="85"/>
+      <c r="F49" s="85"/>
+      <c r="G49" s="85"/>
+      <c r="H49" s="85"/>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B50" s="29"/>
+      <c r="C50" s="29"/>
+      <c r="D50" s="29"/>
+      <c r="E50" s="85"/>
+      <c r="F50" s="85"/>
+      <c r="G50" s="85"/>
+      <c r="H50" s="85"/>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B51" s="29"/>
+      <c r="C51" s="29"/>
+      <c r="D51" s="29"/>
+      <c r="E51" s="85"/>
+      <c r="F51" s="85"/>
+      <c r="G51" s="85"/>
+      <c r="H51" s="85"/>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B52" s="29"/>
+      <c r="C52" s="29"/>
+      <c r="D52" s="29"/>
+      <c r="E52" s="85"/>
+      <c r="F52" s="85"/>
+      <c r="G52" s="85"/>
+      <c r="H52" s="85"/>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B53" s="29"/>
+      <c r="C53" s="29"/>
+      <c r="D53" s="29"/>
+      <c r="E53" s="85"/>
+      <c r="F53" s="85"/>
+      <c r="G53" s="85"/>
+      <c r="H53" s="85"/>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B54" s="29"/>
+      <c r="C54" s="29"/>
+      <c r="D54" s="29"/>
+      <c r="E54" s="85"/>
+      <c r="F54" s="85"/>
+      <c r="G54" s="85"/>
+      <c r="H54" s="85"/>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B55" s="29"/>
+      <c r="C55" s="29"/>
+      <c r="D55" s="29"/>
+      <c r="E55" s="85"/>
+      <c r="F55" s="85"/>
+      <c r="G55" s="85"/>
+      <c r="H55" s="85"/>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B56" s="29"/>
+      <c r="C56" s="29"/>
+      <c r="D56" s="29"/>
+      <c r="E56" s="85"/>
+      <c r="F56" s="85"/>
+      <c r="G56" s="85"/>
+      <c r="H56" s="85"/>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B57" s="29"/>
+      <c r="C57" s="29"/>
+      <c r="D57" s="29"/>
+      <c r="E57" s="85"/>
+      <c r="F57" s="85"/>
+      <c r="G57" s="85"/>
+      <c r="H57" s="85"/>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B58" s="29"/>
+      <c r="C58" s="29"/>
+      <c r="D58" s="29"/>
+      <c r="E58" s="85"/>
+      <c r="F58" s="85"/>
+      <c r="G58" s="85"/>
+      <c r="H58" s="85"/>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B59" s="29"/>
+      <c r="C59" s="29"/>
+      <c r="D59" s="29"/>
+      <c r="E59" s="85"/>
+      <c r="F59" s="85"/>
+      <c r="G59" s="85"/>
+      <c r="H59" s="85"/>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B60" s="29"/>
+      <c r="C60" s="29"/>
+      <c r="D60" s="29"/>
+      <c r="E60" s="85"/>
+      <c r="F60" s="85"/>
+      <c r="G60" s="85"/>
+      <c r="H60" s="85"/>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B61" s="29"/>
+      <c r="C61" s="29"/>
+      <c r="D61" s="29"/>
+      <c r="E61" s="85"/>
+      <c r="F61" s="85"/>
+      <c r="G61" s="85"/>
+      <c r="H61" s="85"/>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B62" s="29"/>
+      <c r="C62" s="29"/>
+      <c r="D62" s="29"/>
+      <c r="E62" s="85"/>
+      <c r="F62" s="85"/>
+      <c r="G62" s="85"/>
+      <c r="H62" s="85"/>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B63" s="29"/>
+      <c r="C63" s="29"/>
+      <c r="D63" s="29"/>
+      <c r="E63" s="85"/>
+      <c r="F63" s="85"/>
+      <c r="G63" s="85"/>
+      <c r="H63" s="85"/>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B64" s="29"/>
+      <c r="C64" s="29"/>
+      <c r="D64" s="29"/>
+      <c r="E64" s="85"/>
+      <c r="F64" s="85"/>
+      <c r="G64" s="85"/>
+      <c r="H64" s="85"/>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B65" s="29"/>
+      <c r="C65" s="29"/>
+      <c r="D65" s="29"/>
+      <c r="E65" s="85"/>
+      <c r="F65" s="85"/>
+      <c r="G65" s="85"/>
+      <c r="H65" s="85"/>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B66" s="29"/>
+      <c r="C66" s="29"/>
+      <c r="D66" s="29"/>
+      <c r="E66" s="85"/>
+      <c r="F66" s="85"/>
+      <c r="G66" s="85"/>
+      <c r="H66" s="85"/>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B67" s="29"/>
+      <c r="C67" s="29"/>
+      <c r="D67" s="29"/>
+      <c r="E67" s="85"/>
+      <c r="F67" s="85"/>
+      <c r="G67" s="85"/>
+      <c r="H67" s="85"/>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B68" s="29"/>
+      <c r="C68" s="29"/>
+      <c r="D68" s="29"/>
+      <c r="E68" s="85"/>
+      <c r="F68" s="85"/>
+      <c r="G68" s="85"/>
+      <c r="H68" s="85"/>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B69" s="29"/>
+      <c r="C69" s="29"/>
+      <c r="D69" s="29"/>
+      <c r="E69" s="85"/>
+      <c r="F69" s="85"/>
+      <c r="G69" s="85"/>
+      <c r="H69" s="85"/>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B70" s="29"/>
+      <c r="C70" s="29"/>
+      <c r="D70" s="29"/>
+      <c r="E70" s="85"/>
+      <c r="F70" s="85"/>
+      <c r="G70" s="85"/>
+      <c r="H70" s="85"/>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B71" s="29"/>
+      <c r="C71" s="29"/>
+      <c r="D71" s="29"/>
+      <c r="E71" s="85"/>
+      <c r="F71" s="85"/>
+      <c r="G71" s="85"/>
+      <c r="H71" s="85"/>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B72" s="28"/>
+      <c r="C72" s="28"/>
+      <c r="D72" s="28"/>
+      <c r="E72" s="85"/>
+      <c r="F72" s="85"/>
+      <c r="G72" s="85"/>
+      <c r="H72" s="85"/>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B73" s="28"/>
+      <c r="C73" s="28"/>
+      <c r="D73" s="28"/>
+      <c r="E73" s="85"/>
+      <c r="F73" s="85"/>
+      <c r="G73" s="85"/>
+      <c r="H73" s="85"/>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B74" s="28"/>
+      <c r="C74" s="28"/>
+      <c r="D74" s="28"/>
+      <c r="E74" s="85"/>
+      <c r="F74" s="85"/>
+      <c r="G74" s="85"/>
+      <c r="H74" s="85"/>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B75" s="28"/>
+      <c r="C75" s="28"/>
+      <c r="D75" s="28"/>
+      <c r="E75" s="85"/>
+      <c r="F75" s="85"/>
+      <c r="G75" s="85"/>
+      <c r="H75" s="85"/>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B76" s="28"/>
+      <c r="C76" s="28"/>
+      <c r="D76" s="28"/>
+      <c r="E76" s="85"/>
+      <c r="F76" s="85"/>
+      <c r="G76" s="85"/>
+      <c r="H76" s="85"/>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B77" s="28"/>
+      <c r="C77" s="28"/>
+      <c r="D77" s="28"/>
+      <c r="E77" s="85"/>
+      <c r="F77" s="85"/>
+      <c r="G77" s="85"/>
+      <c r="H77" s="85"/>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B78" s="28"/>
+      <c r="C78" s="28"/>
+      <c r="D78" s="28"/>
+      <c r="E78" s="85"/>
+      <c r="F78" s="85"/>
+      <c r="G78" s="85"/>
+      <c r="H78" s="85"/>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B79" s="28"/>
+      <c r="C79" s="28"/>
+      <c r="D79" s="28"/>
+      <c r="E79" s="85"/>
+      <c r="F79" s="85"/>
+      <c r="G79" s="85"/>
+      <c r="H79" s="85"/>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B80" s="28"/>
+      <c r="C80" s="28"/>
+      <c r="D80" s="28"/>
+      <c r="E80" s="85"/>
+      <c r="F80" s="85"/>
+      <c r="G80" s="85"/>
+      <c r="H80" s="85"/>
+    </row>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B81" s="28"/>
+      <c r="C81" s="28"/>
+      <c r="D81" s="28"/>
+      <c r="E81" s="85"/>
+      <c r="F81" s="85"/>
+      <c r="G81" s="85"/>
+      <c r="H81" s="85"/>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B82" s="28"/>
+      <c r="C82" s="28"/>
+      <c r="D82" s="28"/>
+      <c r="E82" s="85"/>
+      <c r="F82" s="85"/>
+      <c r="G82" s="85"/>
+      <c r="H82" s="85"/>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B83" s="28"/>
+      <c r="C83" s="28"/>
+      <c r="D83" s="28"/>
+      <c r="E83" s="85"/>
+      <c r="F83" s="85"/>
+      <c r="G83" s="85"/>
+      <c r="H83" s="85"/>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B84" s="28"/>
+      <c r="C84" s="28"/>
+      <c r="D84" s="28"/>
+      <c r="E84" s="85"/>
+      <c r="F84" s="85"/>
+      <c r="G84" s="85"/>
+      <c r="H84" s="85"/>
+    </row>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B85" s="28"/>
+      <c r="C85" s="28"/>
+      <c r="D85" s="28"/>
+      <c r="E85" s="85"/>
+      <c r="F85" s="85"/>
+      <c r="G85" s="85"/>
+      <c r="H85" s="85"/>
+    </row>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B86" s="28"/>
+      <c r="C86" s="28"/>
+      <c r="D86" s="28"/>
+      <c r="E86" s="85"/>
+      <c r="F86" s="85"/>
+      <c r="G86" s="85"/>
+      <c r="H86" s="85"/>
+    </row>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B87" s="28"/>
+      <c r="C87" s="28"/>
+      <c r="D87" s="28"/>
+      <c r="E87" s="85"/>
+      <c r="F87" s="85"/>
+      <c r="G87" s="85"/>
+      <c r="H87" s="85"/>
+    </row>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B88" s="28"/>
+      <c r="C88" s="28"/>
+      <c r="D88" s="28"/>
+      <c r="E88" s="85"/>
+      <c r="F88" s="85"/>
+      <c r="G88" s="85"/>
+      <c r="H88" s="85"/>
+    </row>
+    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B89" s="28"/>
+      <c r="C89" s="28"/>
+      <c r="D89" s="28"/>
+      <c r="E89" s="85"/>
+      <c r="F89" s="85"/>
+      <c r="G89" s="85"/>
+      <c r="H89" s="85"/>
+    </row>
+    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B90" s="28"/>
+      <c r="C90" s="28"/>
+      <c r="D90" s="28"/>
+      <c r="E90" s="85"/>
+      <c r="F90" s="85"/>
+      <c r="G90" s="85"/>
+      <c r="H90" s="85"/>
+    </row>
+    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B91" s="28"/>
+      <c r="C91" s="28"/>
+      <c r="D91" s="28"/>
+      <c r="E91" s="85"/>
+      <c r="F91" s="85"/>
+      <c r="G91" s="85"/>
+      <c r="H91" s="85"/>
+    </row>
+    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B92" s="28"/>
+      <c r="C92" s="28"/>
+      <c r="D92" s="28"/>
+      <c r="E92" s="85"/>
+      <c r="F92" s="85"/>
+      <c r="G92" s="85"/>
+      <c r="H92" s="85"/>
+    </row>
+    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B93" s="28"/>
+      <c r="C93" s="28"/>
+      <c r="D93" s="28"/>
+      <c r="E93" s="85"/>
+      <c r="F93" s="85"/>
+      <c r="G93" s="85"/>
+      <c r="H93" s="85"/>
+    </row>
+    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B94" s="28"/>
+      <c r="C94" s="28"/>
+      <c r="D94" s="28"/>
+      <c r="E94" s="85"/>
+      <c r="F94" s="85"/>
+      <c r="G94" s="85"/>
+      <c r="H94" s="85"/>
+    </row>
+    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B95" s="28"/>
+      <c r="C95" s="28"/>
+      <c r="D95" s="28"/>
+      <c r="E95" s="85"/>
+      <c r="F95" s="85"/>
+      <c r="G95" s="85"/>
+      <c r="H95" s="85"/>
+    </row>
+    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B96" s="28"/>
+      <c r="C96" s="28"/>
+      <c r="D96" s="28"/>
+      <c r="E96" s="85"/>
+      <c r="F96" s="85"/>
+      <c r="G96" s="85"/>
+      <c r="H96" s="85"/>
+    </row>
+    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B97" s="28"/>
+      <c r="C97" s="28"/>
+      <c r="D97" s="28"/>
+      <c r="E97" s="85"/>
+      <c r="F97" s="85"/>
+      <c r="G97" s="85"/>
+      <c r="H97" s="85"/>
+    </row>
+    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B98" s="28"/>
+      <c r="C98" s="28"/>
+      <c r="D98" s="28"/>
+      <c r="E98" s="85"/>
+      <c r="F98" s="85"/>
+      <c r="G98" s="85"/>
+      <c r="H98" s="85"/>
+    </row>
+    <row r="99" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B99" s="28"/>
+      <c r="C99" s="28"/>
+      <c r="D99" s="28"/>
+      <c r="E99" s="85"/>
+      <c r="F99" s="85"/>
+      <c r="G99" s="85"/>
+      <c r="H99" s="85"/>
+    </row>
+    <row r="100" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B100" s="28"/>
+      <c r="C100" s="28"/>
+      <c r="D100" s="28"/>
+      <c r="E100" s="85"/>
+      <c r="F100" s="85"/>
+      <c r="G100" s="85"/>
+      <c r="H100" s="85"/>
+    </row>
+    <row r="101" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B101" s="28"/>
+      <c r="C101" s="28"/>
+      <c r="D101" s="28"/>
+      <c r="E101" s="85"/>
+      <c r="F101" s="85"/>
+      <c r="G101" s="85"/>
+      <c r="H101" s="85"/>
+    </row>
+    <row r="102" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B102" s="28"/>
+      <c r="C102" s="28"/>
+      <c r="D102" s="28"/>
+      <c r="E102" s="85"/>
+      <c r="F102" s="85"/>
+      <c r="G102" s="85"/>
+      <c r="H102" s="85"/>
+    </row>
+    <row r="103" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B103" s="28"/>
+      <c r="C103" s="28"/>
+      <c r="D103" s="28"/>
+      <c r="E103" s="85"/>
+      <c r="F103" s="85"/>
+      <c r="G103" s="85"/>
+      <c r="H103" s="85"/>
+    </row>
+    <row r="104" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B104" s="28"/>
+      <c r="C104" s="28"/>
+      <c r="D104" s="28"/>
+      <c r="E104" s="85"/>
+      <c r="F104" s="85"/>
+      <c r="G104" s="85"/>
+      <c r="H104" s="85"/>
+    </row>
+    <row r="105" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B105" s="28"/>
+      <c r="C105" s="28"/>
+      <c r="D105" s="28"/>
+      <c r="E105" s="85"/>
+      <c r="F105" s="85"/>
+      <c r="G105" s="85"/>
+      <c r="H105" s="85"/>
+    </row>
+    <row r="106" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B106" s="28"/>
+      <c r="C106" s="28"/>
+      <c r="D106" s="28"/>
+      <c r="E106" s="85"/>
+      <c r="F106" s="85"/>
+      <c r="G106" s="85"/>
+      <c r="H106" s="85"/>
+    </row>
+    <row r="107" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B107" s="28"/>
+      <c r="C107" s="28"/>
+      <c r="D107" s="28"/>
+      <c r="E107" s="85"/>
+      <c r="F107" s="85"/>
+      <c r="G107" s="85"/>
+      <c r="H107" s="85"/>
+    </row>
+    <row r="108" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B108" s="28"/>
+      <c r="C108" s="28"/>
+      <c r="D108" s="28"/>
+      <c r="E108" s="85"/>
+      <c r="F108" s="85"/>
+      <c r="G108" s="85"/>
+      <c r="H108" s="85"/>
+    </row>
+    <row r="109" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E109" s="30"/>
+      <c r="F109" s="30"/>
+      <c r="G109" s="30"/>
+      <c r="H109" s="30"/>
+    </row>
+    <row r="110" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E110" s="30"/>
+      <c r="F110" s="30"/>
+      <c r="G110" s="30"/>
+      <c r="H110" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="106">
+    <mergeCell ref="E27:H27"/>
+    <mergeCell ref="E28:H28"/>
+    <mergeCell ref="E29:H29"/>
+    <mergeCell ref="E30:H30"/>
+    <mergeCell ref="E31:H31"/>
+    <mergeCell ref="E32:H32"/>
+    <mergeCell ref="E33:H33"/>
+    <mergeCell ref="E34:H34"/>
+    <mergeCell ref="E35:H35"/>
+    <mergeCell ref="E37:H37"/>
+    <mergeCell ref="E38:H38"/>
+    <mergeCell ref="E39:H39"/>
+    <mergeCell ref="E106:H106"/>
+    <mergeCell ref="E107:H107"/>
+    <mergeCell ref="E108:H108"/>
+    <mergeCell ref="E109:H109"/>
+    <mergeCell ref="E110:H110"/>
+    <mergeCell ref="E101:H101"/>
+    <mergeCell ref="E102:H102"/>
+    <mergeCell ref="E103:H103"/>
+    <mergeCell ref="E104:H104"/>
+    <mergeCell ref="E105:H105"/>
+    <mergeCell ref="E96:H96"/>
+    <mergeCell ref="E97:H97"/>
+    <mergeCell ref="E98:H98"/>
+    <mergeCell ref="E99:H99"/>
+    <mergeCell ref="E100:H100"/>
+    <mergeCell ref="E91:H91"/>
+    <mergeCell ref="E92:H92"/>
+    <mergeCell ref="E93:H93"/>
+    <mergeCell ref="E94:H94"/>
+    <mergeCell ref="E95:H95"/>
+    <mergeCell ref="E86:H86"/>
+    <mergeCell ref="E87:H87"/>
+    <mergeCell ref="E88:H88"/>
+    <mergeCell ref="E89:H89"/>
+    <mergeCell ref="E90:H90"/>
+    <mergeCell ref="E81:H81"/>
+    <mergeCell ref="E82:H82"/>
+    <mergeCell ref="E83:H83"/>
+    <mergeCell ref="E84:H84"/>
+    <mergeCell ref="E85:H85"/>
+    <mergeCell ref="E76:H76"/>
+    <mergeCell ref="E77:H77"/>
+    <mergeCell ref="E78:H78"/>
+    <mergeCell ref="E79:H79"/>
+    <mergeCell ref="E80:H80"/>
+    <mergeCell ref="E71:H71"/>
+    <mergeCell ref="E72:H72"/>
+    <mergeCell ref="E73:H73"/>
+    <mergeCell ref="E74:H74"/>
+    <mergeCell ref="E75:H75"/>
+    <mergeCell ref="E66:H66"/>
+    <mergeCell ref="E67:H67"/>
+    <mergeCell ref="E68:H68"/>
+    <mergeCell ref="E69:H69"/>
+    <mergeCell ref="E70:H70"/>
+    <mergeCell ref="E61:H61"/>
+    <mergeCell ref="E62:H62"/>
+    <mergeCell ref="E63:H63"/>
+    <mergeCell ref="E64:H64"/>
+    <mergeCell ref="E65:H65"/>
+    <mergeCell ref="E56:H56"/>
+    <mergeCell ref="E57:H57"/>
+    <mergeCell ref="E58:H58"/>
+    <mergeCell ref="E59:H59"/>
+    <mergeCell ref="E60:H60"/>
+    <mergeCell ref="E51:H51"/>
+    <mergeCell ref="E52:H52"/>
+    <mergeCell ref="E53:H53"/>
+    <mergeCell ref="E54:H54"/>
+    <mergeCell ref="E55:H55"/>
+    <mergeCell ref="E46:H46"/>
+    <mergeCell ref="E47:H47"/>
+    <mergeCell ref="E48:H48"/>
+    <mergeCell ref="E49:H49"/>
+    <mergeCell ref="E50:H50"/>
+    <mergeCell ref="E41:H41"/>
+    <mergeCell ref="E42:H42"/>
+    <mergeCell ref="E43:H43"/>
+    <mergeCell ref="E44:H44"/>
+    <mergeCell ref="E45:H45"/>
+    <mergeCell ref="E40:H40"/>
+    <mergeCell ref="E26:H26"/>
     <mergeCell ref="E23:H23"/>
     <mergeCell ref="E24:H24"/>
     <mergeCell ref="E25:H25"/>
@@ -1894,10 +2736,10 @@
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="E2:P2"/>
     <mergeCell ref="E3:P3"/>
-    <mergeCell ref="N5:N7"/>
+    <mergeCell ref="O5:O7"/>
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="J7:L9"/>
-    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="K7:M9"/>
+    <mergeCell ref="I5:J5"/>
     <mergeCell ref="E15:H15"/>
     <mergeCell ref="E14:H14"/>
     <mergeCell ref="E16:H16"/>
@@ -1906,7 +2748,8 @@
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B17:D17"/>
-    <mergeCell ref="H7:I9"/>
+    <mergeCell ref="I7:J9"/>
+    <mergeCell ref="E36:H36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>